<commit_message>
Updated datasets for 10250_0020, 10450_0270 and 10550_0270.
</commit_message>
<xml_diff>
--- a/10250_0020.xlsx
+++ b/10250_0020.xlsx
@@ -4242,256 +4242,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId165"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>430</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="166" name="Image 166" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId166"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>0</colOff>
-      <row>430</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="167" name="Image 167" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId167"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>430</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="168" name="Image 168" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId168"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>13</col>
-      <colOff>0</colOff>
-      <row>430</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="169" name="Image 169" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId169"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>17</col>
-      <colOff>0</colOff>
-      <row>430</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="170" name="Image 170" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId170"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>443</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="171" name="Image 171" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId171"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>0</colOff>
-      <row>443</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="172" name="Image 172" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId172"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>443</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="173" name="Image 173" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId173"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>13</col>
-      <colOff>0</colOff>
-      <row>443</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="174" name="Image 174" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId174"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>17</col>
-      <colOff>0</colOff>
-      <row>443</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="175" name="Image 175" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId175"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4794,7 +4544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6265,92 +6015,6 @@
       <c r="I34" t="inlineStr">
         <is>
           <t>cuts/103.0009314,0.5847422_10250_0020_Azul-3.5micras.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>102.8169608_0.3111770_10250_0020_34</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>102.8169608</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.311177</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>cuts/102.8169608,0.3111770_10250_0020_RGB-composite.jpeg</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>cuts/102.8169608,0.3111770_10250_0020_Rojo-8micras.jpeg</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>cuts/102.8169608,0.3111770_10250_0020_I3-5.8micras.jpeg</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>cuts/102.8169608,0.3111770_10250_0020_Verde-4.6micras.jpeg</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>cuts/102.8169608,0.3111770_10250_0020_Azul-3.5micras.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>102.8170056_0.3112443_10250_0020_35</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>102.8170056</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0.3112443</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>cuts/102.8170056,0.3112443_10250_0020_RGB-composite.jpeg</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>cuts/102.8170056,0.3112443_10250_0020_Rojo-8micras.jpeg</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>cuts/102.8170056,0.3112443_10250_0020_I3-5.8micras.jpeg</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>cuts/102.8170056,0.3112443_10250_0020_Verde-4.6micras.jpeg</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>cuts/102.8170056,0.3112443_10250_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
@@ -6365,7 +6029,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R444"/>
+  <dimension ref="A1:R418"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6648,20 +6312,6 @@
         </is>
       </c>
     </row>
-    <row r="431">
-      <c r="A431" t="inlineStr">
-        <is>
-          <t>102.8169608_0.3111770_10250_0020_34</t>
-        </is>
-      </c>
-    </row>
-    <row r="444">
-      <c r="A444" t="inlineStr">
-        <is>
-          <t>102.8170056_0.3112443_10250_0020_35</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>